<commit_message>
import updated algorithm and its integration to requests
</commit_message>
<xml_diff>
--- a/springConverter/src/main/resources/UploadedFiles/result.xlsx
+++ b/springConverter/src/main/resources/UploadedFiles/result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Programming\Java\FilesConverterAlfaBank\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EF9383-DD99-47B2-8A4F-3C9E7AA11772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CA449D-E266-417D-9BC4-2DF100627228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5570" yWindow="790" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="нужный формат" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="24">
   <si>
     <t>Фамилия</t>
   </si>
@@ -97,12 +97,6 @@
   </si>
   <si>
     <t>Псков, 8 Марта, 23</t>
-  </si>
-  <si>
-    <t>Тест дата</t>
-  </si>
-  <si>
-    <t>Тест время</t>
   </si>
 </sst>
 </file>
@@ -446,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:N210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,11 +502,1050 @@
       <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" t="s">
-        <v>25</v>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>